<commit_message>
modified graphs and some logs
</commit_message>
<xml_diff>
--- a/logs/graphs_long.xlsx
+++ b/logs/graphs_long.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16280" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>NODE</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>NODES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A </t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -1087,17 +1096,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>Model</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
               <a:t> execution time for 10seconds simulation</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="2000"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1149,13 +1158,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>SCHEDULE A</c:v>
+                  <c:v>A </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SCHEDULE B</c:v>
+                  <c:v>B</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>SCHEDULE C</c:v>
+                  <c:v>C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1205,6 +1214,50 @@
               </a:ln>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00804597701149425"/>
+                  <c:y val="-0.0254041570438799"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800"/>
+                      <a:t>*</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet3!$B$11:$D$11</c:f>
@@ -1259,6 +1312,61 @@
               </a:ln>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00919540229885057"/>
+                  <c:y val="-0.0138568129330254"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800"/>
+                      <a:t>*</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet3!$B$12:$D$12</c:f>
@@ -1456,6 +1564,25 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Schedules</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1485,6 +1612,25 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1606,15 +1752,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2403,8 +2549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2495,13 +2641,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>1</v>

</xml_diff>